<commit_message>
2022-03-18-vuejs can download django Excel & get All Folder File
</commit_message>
<xml_diff>
--- a/backend/frontend/public/excel_folder/Test.xlsx
+++ b/backend/frontend/public/excel_folder/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Code\project\ExcelSystem\backend\frontend\public\excel_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D156A628-F2C1-47EF-811D-DEA2BD33089F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92536878-8AD8-4355-A1CF-2A78E47AFB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="57">
   <si>
     <t>工程名稱</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -250,14 +250,6 @@
   </si>
   <si>
     <t>圓池外填土整地、循環池配置管路組裝及池內整地夯實</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>NaN</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>NaN</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1065,6 +1057,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1120,12 +1118,6 @@
     <xf numFmtId="179" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1482,10 +1474,10 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="68"/>
+      <c r="A2" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="70"/>
       <c r="C2" s="23" t="s">
         <v>47</v>
       </c>
@@ -1493,24 +1485,24 @@
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="78">
-        <v>1</v>
-      </c>
-      <c r="I2" s="78"/>
+      <c r="H2" s="80">
+        <v>1</v>
+      </c>
+      <c r="I2" s="80"/>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
       <c r="L2" s="24"/>
       <c r="M2" s="24"/>
       <c r="N2" s="24"/>
-      <c r="O2" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="75" t="s">
+      <c r="O2" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="76"/>
-      <c r="S2" s="77"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="79"/>
       <c r="T2" s="2"/>
       <c r="U2" s="4"/>
       <c r="V2" s="5" t="s">
@@ -1522,10 +1514,10 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="27.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="70"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="25" t="s">
         <v>5</v>
       </c>
@@ -1542,13 +1534,13 @@
       <c r="N3" s="26"/>
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
-      <c r="Q3" s="71" t="s">
+      <c r="Q3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="72"/>
-      <c r="S3" s="52" t="e">
+      <c r="R3" s="74"/>
+      <c r="S3" s="52">
         <f>SUMPRODUCT(B6:B23,S6:S23)</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="7" t="s">
@@ -1573,34 +1565,34 @@
         <v>11</v>
       </c>
       <c r="D4" s="43"/>
-      <c r="E4" s="65">
+      <c r="E4" s="67">
         <v>44634</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="65">
+      <c r="F4" s="68"/>
+      <c r="G4" s="67">
         <v>44635</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="65">
+      <c r="H4" s="68"/>
+      <c r="I4" s="67">
         <v>44636</v>
       </c>
-      <c r="J4" s="66"/>
-      <c r="K4" s="65">
+      <c r="J4" s="68"/>
+      <c r="K4" s="67">
         <v>44637</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="65">
+      <c r="L4" s="68"/>
+      <c r="M4" s="67">
         <v>44638</v>
       </c>
-      <c r="N4" s="66"/>
-      <c r="O4" s="65">
+      <c r="N4" s="68"/>
+      <c r="O4" s="67">
         <v>44639</v>
       </c>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="65">
+      <c r="P4" s="68"/>
+      <c r="Q4" s="67">
         <v>44640</v>
       </c>
-      <c r="R4" s="66"/>
+      <c r="R4" s="68"/>
       <c r="S4" s="53" t="s">
         <v>50</v>
       </c>
@@ -1736,16 +1728,16 @@
         <f>IF(O6/$D$6="- ",0,O6/$D$6)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R6" s="40" t="e">
+      <c r="Q6" s="20">
+        <v>1</v>
+      </c>
+      <c r="R6" s="40">
         <f>IF(Q6/$D$6="- ",0,Q6/$D$6)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S6" s="55" t="e">
+        <v>2.1739130434782608E-2</v>
+      </c>
+      <c r="S6" s="55">
         <f>MAX(F6,H6,J6,L6,N6,P6,R6)</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T6" s="2"/>
       <c r="U6" s="13" t="s">
@@ -1812,16 +1804,16 @@
         <f>IF(O7/$D$7="- ",0,O7/$D$7)</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R7" s="40" t="e">
+      <c r="Q7" s="20">
+        <v>1</v>
+      </c>
+      <c r="R7" s="40">
         <f>IF(Q7/$D$7="- ",0,Q7/$D$7)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S7" s="55" t="e">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S7" s="55">
         <f t="shared" ref="S7:S27" si="0">MAX(F7,H7,J7,L7,N7,P7,R7)</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
@@ -1884,16 +1876,16 @@
         <f>IF(O8/$D$8="- ",0,O8/$D$8)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R8" s="40" t="e">
+      <c r="Q8" s="20">
+        <v>1</v>
+      </c>
+      <c r="R8" s="40">
         <f>IF(Q8/$D$8="- ",0,Q8/$D$8)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S8" s="55" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="S8" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="15" t="s">
@@ -1960,16 +1952,16 @@
         <f>IF(O9/$D$9="- ",0,O9/$D$9)</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R9" s="40" t="e">
+      <c r="Q9" s="20">
+        <v>1</v>
+      </c>
+      <c r="R9" s="40">
         <f>IF(Q9/$D$9="- ",0,Q9/$D$9)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S9" s="55" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="S9" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
@@ -2032,16 +2024,16 @@
         <f>IF(O10/$D$10="- ",0,O10/$D$10)</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R10" s="40" t="e">
+      <c r="Q10" s="20">
+        <v>1</v>
+      </c>
+      <c r="R10" s="40">
         <f>IF(Q10/$D$10="- ",0,Q10/$D$10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S10" s="55" t="e">
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="S10" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
@@ -2104,16 +2096,16 @@
         <f>IF(O11/$D$11="- ",0,O11/$D$11)</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R11" s="40" t="e">
+      <c r="Q11" s="20">
+        <v>1</v>
+      </c>
+      <c r="R11" s="40">
         <f>IF(Q11/$D$11="- ",0,Q11/$D$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S11" s="55" t="e">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="S11" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -2176,16 +2168,16 @@
         <f>IF(O12/$D$12="- ",0,O12/$D$12)</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R12" s="40" t="e">
+      <c r="Q12" s="20">
+        <v>1</v>
+      </c>
+      <c r="R12" s="40">
         <f>IF(Q12/$D$12="- ",0,Q12/$D$12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S12" s="55" t="e">
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="S12" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
@@ -2248,16 +2240,16 @@
         <f>IF(O13/$D$13="- ",0,O13/$D$13)</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R13" s="40" t="e">
+      <c r="Q13" s="20">
+        <v>1</v>
+      </c>
+      <c r="R13" s="40">
         <f>IF(Q13/$D$13="- ",0,Q13/$D$13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S13" s="55" t="e">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="S13" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
@@ -2320,16 +2312,16 @@
         <f>IF(O14/$D$14="- ",0,O14/$D$14)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R14" s="40" t="e">
+      <c r="Q14" s="20">
+        <v>1</v>
+      </c>
+      <c r="R14" s="40">
         <f>IF(Q14/$D$14="- ",0,Q14/$D$14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S14" s="55" t="e">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="S14" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
@@ -2392,16 +2384,16 @@
         <f>IF(O15/$D$15="- ",0,O15/$D$15)</f>
         <v>0</v>
       </c>
-      <c r="Q15" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R15" s="40" t="e">
+      <c r="Q15" s="20">
+        <v>1</v>
+      </c>
+      <c r="R15" s="40">
         <f>IF(Q15/$D$15="- ",0,Q15/$D$15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S15" s="55" t="e">
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="S15" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
@@ -2464,16 +2456,16 @@
         <f>IF(O16/$D$16="- ",0,O16/$D$16)</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R16" s="40" t="e">
+      <c r="Q16" s="20">
+        <v>1</v>
+      </c>
+      <c r="R16" s="40">
         <f>IF(Q16/$D$16="- ",0,Q16/$D$16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S16" s="55" t="e">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="S16" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
@@ -2536,16 +2528,16 @@
         <f>IF(O17/$D$17="- ",0,O17/$D$17)</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R17" s="40" t="e">
+      <c r="Q17" s="20">
+        <v>1</v>
+      </c>
+      <c r="R17" s="40">
         <f>IF(Q17/$D$17="- ",0,Q17/$D$17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S17" s="55" t="e">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="S17" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
@@ -2608,16 +2600,16 @@
         <f>IF(O18/$D$18="- ",0,O18/$D$18)</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R18" s="40" t="e">
+      <c r="Q18" s="20">
+        <v>1</v>
+      </c>
+      <c r="R18" s="40">
         <f>IF(Q18/$D$18="- ",0,Q18/$D$18)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S18" s="55" t="e">
+        <v>1</v>
+      </c>
+      <c r="S18" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
@@ -2680,16 +2672,16 @@
         <f>IF(O19/$D$19="- ",0,O19/$D$19)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R19" s="40" t="e">
+      <c r="Q19" s="20">
+        <v>1</v>
+      </c>
+      <c r="R19" s="40">
         <f>IF(Q19/$D$19="- ",0,Q19/$D$19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S19" s="55" t="e">
+        <v>1</v>
+      </c>
+      <c r="S19" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
@@ -2752,16 +2744,16 @@
         <f>IF(O20/$D$20="- ",0,O20/$D$20)</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R20" s="40" t="e">
+      <c r="Q20" s="20">
+        <v>1</v>
+      </c>
+      <c r="R20" s="40">
         <f>IF(Q20/$D$20="- ",0,Q20/$D$20)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S20" s="55" t="e">
+        <v>1</v>
+      </c>
+      <c r="S20" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
@@ -2824,16 +2816,16 @@
         <f>IF(O21/$D$21="- ",0,O21/$D$21)</f>
         <v>0</v>
       </c>
-      <c r="Q21" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R21" s="40" t="e">
+      <c r="Q21" s="20">
+        <v>1</v>
+      </c>
+      <c r="R21" s="40">
         <f>IF(Q21/$D$21="- ",0,Q21/$D$21)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S21" s="55" t="e">
+        <v>0.125</v>
+      </c>
+      <c r="S21" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
@@ -2896,16 +2888,16 @@
         <f>IF(O22/$D$22="- ",0,O22/$D$22)</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R22" s="40" t="e">
+      <c r="Q22" s="20">
+        <v>1</v>
+      </c>
+      <c r="R22" s="40">
         <f>IF(Q22/$D$22="- ",0,Q22/$D$22)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S22" s="55" t="e">
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="S22" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
@@ -2968,16 +2960,16 @@
         <f>IF(O23/$D$23="- ",0,O23/$D$23)</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="R23" s="40" t="e">
+      <c r="Q23" s="20">
+        <v>1</v>
+      </c>
+      <c r="R23" s="40">
         <f>IF(Q23/$D$23="- ",0,Q23/$D$23)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S23" s="55" t="e">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="S23" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
@@ -3040,9 +3032,9 @@
       <c r="R24" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="S24" s="52" t="e">
+      <c r="S24" s="52">
         <f>SUMPRODUCT(B25:B27,S25:S27)</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
@@ -3105,16 +3097,16 @@
         <f>IF(O25/$D$25="- ",0,O25/$D$25)</f>
         <v>0</v>
       </c>
-      <c r="Q25" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="R25" s="40" t="e">
+      <c r="Q25" s="21">
+        <v>1</v>
+      </c>
+      <c r="R25" s="40">
         <f>IF(Q25/$D$25="- ",0,Q25/$D$25)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S25" s="55" t="e">
+        <v>2.0876826722338203E-3</v>
+      </c>
+      <c r="S25" s="55">
         <f>MAX(F25,H25,J25,L25,N25,P25,R25)</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
@@ -3177,16 +3169,16 @@
         <f>IF(O26/$D$26="- ",0,O26/$D$26)</f>
         <v>0</v>
       </c>
-      <c r="Q26" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="R26" s="40" t="e">
+      <c r="Q26" s="21">
+        <v>1</v>
+      </c>
+      <c r="R26" s="40">
         <f>IF(Q26/$D$26="- ",0,Q26/$D$26)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S26" s="55" t="e">
+        <v>2.0876826722338203E-3</v>
+      </c>
+      <c r="S26" s="55">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
@@ -3249,16 +3241,16 @@
         <f>IF(O27/$D$27="- ",0,O27/$D$27)</f>
         <v>0</v>
       </c>
-      <c r="Q27" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="R27" s="58" t="e">
+      <c r="Q27" s="22">
+        <v>1</v>
+      </c>
+      <c r="R27" s="58">
         <f>IF(Q27/$D$27="- ",0,Q27/$D$27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S27" s="59" t="e">
+        <v>2.0876826722338203E-3</v>
+      </c>
+      <c r="S27" s="59">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
@@ -3277,31 +3269,24 @@
         <v>53</v>
       </c>
       <c r="D28" s="61"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="80"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="80"/>
-      <c r="O28" s="79"/>
-      <c r="P28" s="80"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="80"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="66"/>
       <c r="S28" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -3315,6 +3300,13 @@
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.1875" right="0.11811023622047245" top="0.47499999999999998" bottom="0.5625" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3367,10 +3359,10 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="68"/>
+      <c r="A2" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="70"/>
       <c r="C2" s="23" t="s">
         <v>48</v>
       </c>
@@ -3378,24 +3370,24 @@
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="78">
-        <v>1</v>
-      </c>
-      <c r="I2" s="78"/>
+      <c r="H2" s="80">
+        <v>1</v>
+      </c>
+      <c r="I2" s="80"/>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
       <c r="L2" s="24"/>
       <c r="M2" s="24"/>
       <c r="N2" s="24"/>
-      <c r="O2" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="75" t="s">
+      <c r="O2" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="76"/>
-      <c r="S2" s="77"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="79"/>
       <c r="T2" s="2"/>
       <c r="U2" s="4"/>
       <c r="V2" s="5" t="s">
@@ -3407,10 +3399,10 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="27.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="70"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="25" t="s">
         <v>5</v>
       </c>
@@ -3427,10 +3419,10 @@
       <c r="N3" s="26"/>
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
-      <c r="Q3" s="71" t="s">
+      <c r="Q3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="72"/>
+      <c r="R3" s="74"/>
       <c r="S3" s="52">
         <f>SUMPRODUCT(B6:B23,S6:S23)</f>
         <v>0.03</v>
@@ -3458,34 +3450,34 @@
         <v>11</v>
       </c>
       <c r="D4" s="43"/>
-      <c r="E4" s="65">
+      <c r="E4" s="67">
         <v>44501</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="65">
+      <c r="F4" s="68"/>
+      <c r="G4" s="67">
         <v>44502</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="65">
+      <c r="H4" s="68"/>
+      <c r="I4" s="67">
         <v>44503</v>
       </c>
-      <c r="J4" s="66"/>
-      <c r="K4" s="65">
+      <c r="J4" s="68"/>
+      <c r="K4" s="67">
         <v>44504</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="65">
+      <c r="L4" s="68"/>
+      <c r="M4" s="67">
         <v>44505</v>
       </c>
-      <c r="N4" s="66"/>
-      <c r="O4" s="65">
+      <c r="N4" s="68"/>
+      <c r="O4" s="67">
         <v>44506</v>
       </c>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="65">
+      <c r="P4" s="68"/>
+      <c r="Q4" s="67">
         <v>44507</v>
       </c>
-      <c r="R4" s="66"/>
+      <c r="R4" s="68"/>
       <c r="S4" s="53" t="s">
         <v>50</v>
       </c>
@@ -4916,31 +4908,24 @@
         <v>53</v>
       </c>
       <c r="D28" s="61"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="80"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="80"/>
-      <c r="O28" s="79"/>
-      <c r="P28" s="80"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="80"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="66"/>
       <c r="S28" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="A2:B2"/>
@@ -4954,6 +4939,13 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.47499999999999998" bottom="0.61250000000000004" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -5005,10 +4997,10 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="68"/>
+      <c r="A2" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="70"/>
       <c r="C2" s="23" t="s">
         <v>49</v>
       </c>
@@ -5016,24 +5008,24 @@
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="78">
-        <v>1</v>
-      </c>
-      <c r="I2" s="78"/>
+      <c r="H2" s="80">
+        <v>1</v>
+      </c>
+      <c r="I2" s="80"/>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
       <c r="L2" s="24"/>
       <c r="M2" s="24"/>
       <c r="N2" s="24"/>
-      <c r="O2" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="75" t="s">
+      <c r="O2" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="76"/>
-      <c r="S2" s="77"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="79"/>
       <c r="T2" s="2"/>
       <c r="U2" s="4"/>
       <c r="V2" s="5" t="s">
@@ -5045,10 +5037,10 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="27.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="70"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="25" t="s">
         <v>5</v>
       </c>
@@ -5065,10 +5057,10 @@
       <c r="N3" s="26"/>
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
-      <c r="Q3" s="71" t="s">
+      <c r="Q3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="72"/>
+      <c r="R3" s="74"/>
       <c r="S3" s="52">
         <f>SUMPRODUCT(B6:B23,S6:S23)</f>
         <v>0.03</v>
@@ -5096,34 +5088,34 @@
         <v>11</v>
       </c>
       <c r="D4" s="43"/>
-      <c r="E4" s="65">
+      <c r="E4" s="67">
         <v>44501</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="65">
+      <c r="F4" s="68"/>
+      <c r="G4" s="67">
         <v>44502</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="65">
+      <c r="H4" s="68"/>
+      <c r="I4" s="67">
         <v>44503</v>
       </c>
-      <c r="J4" s="66"/>
-      <c r="K4" s="65">
+      <c r="J4" s="68"/>
+      <c r="K4" s="67">
         <v>44504</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="65">
+      <c r="L4" s="68"/>
+      <c r="M4" s="67">
         <v>44505</v>
       </c>
-      <c r="N4" s="66"/>
-      <c r="O4" s="65">
+      <c r="N4" s="68"/>
+      <c r="O4" s="67">
         <v>44506</v>
       </c>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="65">
+      <c r="P4" s="68"/>
+      <c r="Q4" s="67">
         <v>44507</v>
       </c>
-      <c r="R4" s="66"/>
+      <c r="R4" s="68"/>
       <c r="S4" s="53" t="s">
         <v>50</v>
       </c>
@@ -6554,31 +6546,24 @@
         <v>53</v>
       </c>
       <c r="D28" s="61"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="80"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="80"/>
-      <c r="O28" s="79"/>
-      <c r="P28" s="80"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="80"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="66"/>
       <c r="S28" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="A2:B2"/>
@@ -6592,6 +6577,13 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.47499999999999998" bottom="0.61250000000000004" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -6644,10 +6636,10 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="68"/>
+      <c r="A2" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="70"/>
       <c r="C2" s="23" t="s">
         <v>16</v>
       </c>
@@ -6655,24 +6647,24 @@
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="78">
-        <v>1</v>
-      </c>
-      <c r="I2" s="78"/>
+      <c r="H2" s="80">
+        <v>1</v>
+      </c>
+      <c r="I2" s="80"/>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
       <c r="L2" s="24"/>
       <c r="M2" s="24"/>
       <c r="N2" s="24"/>
-      <c r="O2" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="75" t="s">
+      <c r="O2" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="76"/>
-      <c r="S2" s="77"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="79"/>
       <c r="T2" s="2"/>
       <c r="U2" s="4"/>
       <c r="V2" s="5" t="s">
@@ -6684,10 +6676,10 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="27.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="70"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="25" t="s">
         <v>5</v>
       </c>
@@ -6704,10 +6696,10 @@
       <c r="N3" s="26"/>
       <c r="O3" s="26"/>
       <c r="P3" s="26"/>
-      <c r="Q3" s="71" t="s">
+      <c r="Q3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="72"/>
+      <c r="R3" s="74"/>
       <c r="S3" s="52">
         <f>SUMPRODUCT(B6:B23,S6:S23)</f>
         <v>0.03</v>
@@ -6735,34 +6727,34 @@
         <v>11</v>
       </c>
       <c r="D4" s="43"/>
-      <c r="E4" s="65">
+      <c r="E4" s="67">
         <v>44501</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="65">
+      <c r="F4" s="68"/>
+      <c r="G4" s="67">
         <v>44502</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="65">
+      <c r="H4" s="68"/>
+      <c r="I4" s="67">
         <v>44503</v>
       </c>
-      <c r="J4" s="66"/>
-      <c r="K4" s="65">
+      <c r="J4" s="68"/>
+      <c r="K4" s="67">
         <v>44504</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="65">
+      <c r="L4" s="68"/>
+      <c r="M4" s="67">
         <v>44505</v>
       </c>
-      <c r="N4" s="66"/>
-      <c r="O4" s="65">
+      <c r="N4" s="68"/>
+      <c r="O4" s="67">
         <v>44506</v>
       </c>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="65">
+      <c r="P4" s="68"/>
+      <c r="Q4" s="67">
         <v>44507</v>
       </c>
-      <c r="R4" s="66"/>
+      <c r="R4" s="68"/>
       <c r="S4" s="53" t="s">
         <v>50</v>
       </c>
@@ -8193,31 +8185,24 @@
         <v>53</v>
       </c>
       <c r="D28" s="61"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="80"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="80"/>
-      <c r="O28" s="79"/>
-      <c r="P28" s="80"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="80"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="66"/>
       <c r="S28" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="A2:B2"/>
@@ -8231,6 +8216,13 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.11811023622047245" right="0.21249999999999999" top="0.47499999999999998" bottom="0.51875000000000004" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>